<commit_message>
1st Update - adding & improvement
1st Update - adding & improvement
</commit_message>
<xml_diff>
--- a/Vendas.xlsx
+++ b/Vendas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keylla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F51C9B-71C0-4CC5-8C3F-BD135457D1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D8882-6679-474E-B210-93120375BA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31575" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -92,16 +92,16 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Programation</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
     <t>Dual</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>WXZ</t>
+  </si>
+  <si>
+    <t>Cia</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -405,7 +405,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -430,7 +430,7 @@
       <c r="F2" s="5">
         <v>340</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -457,7 +457,7 @@
       <c r="F3" s="5">
         <v>300</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -484,7 +484,7 @@
       <c r="F4" s="5">
         <v>150</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -511,7 +511,7 @@
       <c r="F5" s="5">
         <v>600</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -538,7 +538,7 @@
       <c r="F6" s="5">
         <v>60</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -565,7 +565,7 @@
       <c r="F7" s="5">
         <v>160</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -581,7 +581,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
@@ -592,7 +592,7 @@
       <c r="F8" s="5">
         <v>600</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -619,7 +619,7 @@
       <c r="F9" s="5">
         <v>240</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -646,7 +646,7 @@
       <c r="F10" s="5">
         <v>400</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -673,7 +673,7 @@
       <c r="F11" s="5">
         <v>60</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -689,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
@@ -700,7 +700,7 @@
       <c r="F12" s="5">
         <v>450</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -727,7 +727,7 @@
       <c r="F13" s="5">
         <v>80</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -754,7 +754,7 @@
       <c r="F14" s="5">
         <v>100</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -781,7 +781,7 @@
       <c r="F15" s="5">
         <v>850</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -808,7 +808,7 @@
       <c r="F16" s="5">
         <v>510</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -835,7 +835,7 @@
       <c r="F17" s="5">
         <v>600</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -862,7 +862,7 @@
       <c r="F18" s="5">
         <v>200</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -889,7 +889,7 @@
       <c r="F19" s="5">
         <v>600</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -916,7 +916,7 @@
       <c r="F20" s="5">
         <v>170</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -943,7 +943,7 @@
       <c r="F21" s="5">
         <v>240</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -970,7 +970,7 @@
       <c r="F22" s="5">
         <v>60</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -997,7 +997,7 @@
       <c r="F23" s="5">
         <v>300</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -1024,7 +1024,7 @@
       <c r="F24" s="5">
         <v>500</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1051,7 +1051,7 @@
       <c r="F25" s="5">
         <v>170</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -1078,7 +1078,7 @@
       <c r="F26" s="5">
         <v>100</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -1105,7 +1105,7 @@
       <c r="F27" s="5">
         <v>200</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1121,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -1132,7 +1132,7 @@
       <c r="F28" s="5">
         <v>300</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -1159,7 +1159,7 @@
       <c r="F29" s="5">
         <v>170</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -1186,7 +1186,7 @@
       <c r="F30" s="5">
         <v>80</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1213,7 +1213,7 @@
       <c r="F31" s="5">
         <v>200</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -1240,7 +1240,7 @@
       <c r="F32" s="5">
         <v>80</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -1267,7 +1267,7 @@
       <c r="F33" s="5">
         <v>100</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -1294,7 +1294,7 @@
       <c r="F34" s="5">
         <v>300</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -1321,7 +1321,7 @@
       <c r="F35" s="5">
         <v>100</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -1348,7 +1348,7 @@
       <c r="F36" s="5">
         <v>400</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1375,7 +1375,7 @@
       <c r="F37" s="5">
         <v>200</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -1402,7 +1402,7 @@
       <c r="F38" s="5">
         <v>200</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -1429,7 +1429,7 @@
       <c r="F39" s="5">
         <v>160</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -1456,7 +1456,7 @@
       <c r="F40" s="5">
         <v>320</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -1483,7 +1483,7 @@
       <c r="F41" s="5">
         <v>400</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -1510,7 +1510,7 @@
       <c r="F42" s="5">
         <v>160</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -1537,7 +1537,7 @@
       <c r="F43" s="5">
         <v>340</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -1546,7 +1546,7 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G44" s="1"/>
+      <c r="G44" s="5"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>

</xml_diff>